<commit_message>
auto complete hp and accounts file and open it to user
</commit_message>
<xml_diff>
--- a/RELAÇÃO DE CONTAS E HISTORICOS FAPERS.xlsx
+++ b/RELAÇÃO DE CONTAS E HISTORICOS FAPERS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\NetBeansProjects\FAPERS_BRPREV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520FC903-183B-49A4-8893-A2A7145DD746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D98CD6-9D10-45AB-9F7E-F536A7B2973A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTAS FAPERS" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="659">
   <si>
     <t>CONTA CONTÁBIL</t>
   </si>
@@ -769,9 +769,6 @@
     <t>ADM-00060/2021 -  EMIT ORC: ADM-00061/2021 - 26/02/2021-10952598-17 - CONCESSAO TRI - VALE TRASPORTE 42 - VALE TRANSPORTE - ASSOC EMPRESAS TRANSPORTES PASSAGEIROS DE POADT COMPET: 26/02/2021</t>
   </si>
   <si>
-    <t>APROPR VALE TRANSPORTE ESTAGIARIOS REF FEV/21</t>
-  </si>
-  <si>
     <t>ADM-01703/2020 -  EMIT ORC: ADM-01704/2020 - 02/02/2021-2100024502-29 - PREST SERVICOS MEDICOS-CO-PARTICIPACAO 36 - PLANO DE SAUDE - EMPREGADOS - UNIMED PORTO ALEGRE SOCIEDADE COOPERATIVA DE TRABALHO MEDICODT COMPET: 02/02/2021</t>
   </si>
   <si>
@@ -793,18 +790,6 @@
     <t>VLR PARCELA 07/12 DA AQUISIÇÃO DE 19 LICENÇAS ANTIVIRUS WF TECNOLOGIA LTDA</t>
   </si>
   <si>
-    <t>VLR TAFIC PGS REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR TAFIC PLANO MISTO REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR TAFIC PBD I REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR TAFIC PREVER REF FEV/21</t>
-  </si>
-  <si>
     <t>VLR PARC 02/12 REF IPTU 2021 CASA 1073 MARCILIO DIAS</t>
   </si>
   <si>
@@ -814,24 +799,6 @@
     <t>ADM-00058/2021 -  EMIT ORC: ADM-00059/2021 - 19/02/2021-27278485-19 - CONCESSAO PAT- VALE REFEICAO 41 - VALE REFEICAO-PATRONAL - TICKET SERVICOS S.A.DT COMPET: 19/02/2021</t>
   </si>
   <si>
-    <t>APROPR TICKET SERV S/A REF ALIMENTAÇÃO MÊS FEV/21</t>
-  </si>
-  <si>
-    <t>APROPR TICKET SERV S/A REF REFEIÇÃO MÊS FEV/21</t>
-  </si>
-  <si>
-    <t>APROPR SEGURO CONSELHO DELIBERATIVO REF FEV/21 CFE APOLICE AIG SEGUROS BRASIL S/A Nº 08737.2020.01.0310.001161</t>
-  </si>
-  <si>
-    <t>APROPR SEGURO DIRIGENTES REF FEV/21 CFE APOLICE AIG SEGUROS BRASIL S/A Nº 08737.2020.01.0310.001161</t>
-  </si>
-  <si>
-    <t>APROPR SEGURO EMPREGADOS REF FEV/21 CFE APOLICE AIG SEGUROS BRASIL S/A Nº 08737.2020.01.0310.001161</t>
-  </si>
-  <si>
-    <t>APROPR SEGURO CONSELHO FISCAL REF FEV/21 CFE APOLICE AIG SEGUROS BRASIL S/A Nº 08737.2020.01.0310.001161</t>
-  </si>
-  <si>
     <t>LIQ PARC CUSTEIO ADM INVEST PLANO MISTO REF JAN/21</t>
   </si>
   <si>
@@ -841,15 +808,6 @@
     <t>LIQ PARC CUSTEIO ADM INVEST PREVER REF JAN/21</t>
   </si>
   <si>
-    <t>VLR FONTE CUSTEIO ADM DOS INVESTIMENTOS PGS REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR FONTE CUSTEIO ADM DOS INVESTIMENTOS PREVER REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR FONTE CUSTEIO ADM DOS INVESTIMENTOS PLANO MISTO REF FEV/21</t>
-  </si>
-  <si>
     <t>VLR RESGATE A RECEBER  NTN-B - BOLETA Nº 723/2012</t>
   </si>
   <si>
@@ -1348,18 +1306,12 @@
     <t>VLR RET IRRF CFE FL PGTO FEV/21</t>
   </si>
   <si>
-    <t>VLR PENSAO ALIMENTICIA CFE FL PAGTO MÊS FEV/21</t>
-  </si>
-  <si>
     <t>VLR RET CONTR FAPERS CFE FL SALARIAL FEV/21</t>
   </si>
   <si>
     <t>VLR DESC VR CFE FL SALARIAL FEV/21</t>
   </si>
   <si>
-    <t>VLR DESC CCA PARTIC PGS CFE FL PGTO FAPERS REF FEV/21</t>
-  </si>
-  <si>
     <t>DESC PARCELA EMPRÉST CFE FL SALARIAL FAPERS N/MÊS</t>
   </si>
   <si>
@@ -1375,33 +1327,12 @@
     <t>CONT-00005/2021 - CONSIGNATARIO - INSS S/ SERVICO - INSS - INSTITUTO NACIONAL DO SEGURO SOCIALDT COMPET: 19/02/2021</t>
   </si>
   <si>
-    <t>APROPR INSS S/ GRATIF RICARDO ALTAIR SCHWARZ REF FEV/21</t>
-  </si>
-  <si>
-    <t>APROPR DE INSS RICARDO ALTAIR SCHWARZ REF FEV/21</t>
-  </si>
-  <si>
-    <t>APROPR DE INSS JOSE PEDRO OSORIO MENDINA REF FEV/21</t>
-  </si>
-  <si>
-    <t>APROPR DE INSS ALVARO ROQUE KERN JUNQUEIRA REF FEV/21</t>
-  </si>
-  <si>
-    <t>APROP INSS CFE FOLHA SALARIAL DE FEV/21</t>
-  </si>
-  <si>
     <t>VLR BX PROV INSS S/FÉRIAS N/MÊS</t>
   </si>
   <si>
     <t>ADM-01628/2020 - 01-2021 - FGTS - CAIXA ECON. FEDERALDT COMPET: 05/02/2021</t>
   </si>
   <si>
-    <t>APROP FGTS CFE FOLHA SALARIAL DE FEV/21</t>
-  </si>
-  <si>
-    <t>VLR AJUSTE CFE FGTS N/MÊS</t>
-  </si>
-  <si>
     <t>VLR BX PROV FGTS S/FÉRIAS N/MÊS</t>
   </si>
   <si>
@@ -1462,21 +1393,6 @@
     <t>VLR LIQ CONTR DA PATROC FAPERS REF ATIVOS P/ PLANO MISTO DE JAN/21</t>
   </si>
   <si>
-    <t>VLR LIQ CCA DA PATROC FAPERS P/ PGS REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR LIQ CCA DA PATROC FAPERS REF ASSISTIDOS P/ PGS DE FEV/21</t>
-  </si>
-  <si>
-    <t>VLR LIQ CONTR DA PATROC FAPERS REF ATIVOS P/ PLANO MISTO DE FEV/21</t>
-  </si>
-  <si>
-    <t>VLR LIQ CCA DA PATROC FAPERS REF ASSISTIDOS P/ PLANO MISTO DE FEV/21</t>
-  </si>
-  <si>
-    <t>VLR LIQ CCA DA PATROC FAPERS P/ PREVER REF FEV/21</t>
-  </si>
-  <si>
     <t>APROPR CONTR ASSISITIDOS PLANO MISTO PATROC FAPERS N/MES</t>
   </si>
   <si>
@@ -1849,24 +1765,6 @@
     <t>ADM-00022/2021 - 25/02/2021-21/006104595-17 - SERV. AGUA E ESGOTO-CONTRATO DMAE 17 - DMAE - DEPARTAMENTO MUNICIPAL DE AGUA E ESGOTOSDT COMPET: 25/02/2021</t>
   </si>
   <si>
-    <t>VLR GRATIF RICARDO ALTAIR SCHWARZ REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR GRATIFJOSE PEDRO OSORIO MENDINA REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR GRATIF ALVARO ROQUE KERN JUNQUEIRA REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR IRRF S/ GRATIF RICARDO ALTAIR SCHWARZ REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR IRRF S/ GRATIF JOSE PEDRO OSORIO MENDINA REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR IRRF S/ GRATIF ALVARO ROQUE KERN JUNQUEIRA REF FEV/21</t>
-  </si>
-  <si>
     <t>ADM-00009/2021 - 02-2021 - PGTO GRATIFICACAO DE REPRESENTACAO - RICARDO ALTAIR SCHWARZDT COMPET: 26/02/2021</t>
   </si>
   <si>
@@ -1969,15 +1867,6 @@
     <t>VLR LIQ CONTR PARTIC ATIVOS DA PATROC FAPERS P/ PLANO MISTO REF JAN/21</t>
   </si>
   <si>
-    <t>VLR LIQ CCA PARTIC ATIVOS DA PATROC FAPERS P/ PGS REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR LIQ CONTR PARTIC ATIVOS DA PATROC FAPERS P/ PLANO MISTO REF FEV/21</t>
-  </si>
-  <si>
-    <t>VLR LIQ CCA PARTIC ATIVOS DA PATROC FAPERS P/ PREVER REF FEV/21</t>
-  </si>
-  <si>
     <t>ADM-00008/2021 - 02-2021 - PGTO PENSAO ALIMENTICIA - ELISANGELA AGUIRRE DOS SANTOSDT COMPET: 26/02/2021</t>
   </si>
   <si>
@@ -2008,10 +1897,118 @@
     <t>APROP AUXILIO EDUCAÇÃO CFE FL SALARIAL FEV/21.</t>
   </si>
   <si>
-    <t>APROPR TICKET SERV S/A REF REFEIÇÃO ESTAGIÁRIOS MÊS FEV/21</t>
-  </si>
-  <si>
     <t xml:space="preserve">Conta Único </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROP INSS CFE FOLHA SALARIAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROP FGTS CFE FOLHA SALARIAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR LIQ CCA DA PATROC FAPERS REF ASSISTIDOS P/ PGS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR LIQ CCA DA PATROC FAPERS REF ASSISTIDOS P/ PLANO MISTO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR LIQ CONTR DA PATROC FAPERS REF ATIVOS P/ PLANO MISTO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR GRATIF RICARDO ALTAIR SCHWARZ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR GRATIFJOSE PEDRO OSORIO MENDINA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR GRATIF ALVARO ROQUE KERN JUNQUEIRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROPR DE INSS RICARDO ALTAIR SCHWARZ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROPR DE INSS JOSE PEDRO OSORIO MENDINA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROPR DE INSS ALVARO ROQUE KERN JUNQUEIRA </t>
+  </si>
+  <si>
+    <t>APROPR SEGURO DIRIGENTES  CFE APOLICE AIG SEGUROS BRASIL S/A Nº 08737.2020.01.0310.001161</t>
+  </si>
+  <si>
+    <t>APROPR SEGURO EMPREGADOS  CFE APOLICE AIG SEGUROS BRASIL S/A Nº 08737.2020.01.0310.001161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR DESC CCA PARTIC PGS CFE FL PGTO FAPERS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR TAFIC PBD I </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR TAFIC PGS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR TAFIC PLANO MISTO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR TAFIC PREVER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROPR VALE TRANSPORTE ESTAGIARIOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROPR INSS S/ GRATIF RICARDO ALTAIR SCHWARZ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR IRRF S/ GRATIF ALVARO ROQUE KERN JUNQUEIRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR IRRF S/ GRATIF JOSE PEDRO OSORIO MENDINA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR IRRF S/ GRATIF RICARDO ALTAIR SCHWARZ </t>
+  </si>
+  <si>
+    <t>APROPR SEGURO CONSELHO DELIBERATIVO  CFE APOLICE AIG SEGUROS BRASIL S/A Nº 08737.2020.01.0310.001161</t>
+  </si>
+  <si>
+    <t>APROPR SEGURO CONSELHO FISCAL  CFE APOLICE AIG SEGUROS BRASIL S/A Nº 08737.2020.01.0310.001161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR FONTE CUSTEIO ADM DOS INVESTIMENTOS PGS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR FONTE CUSTEIO ADM DOS INVESTIMENTOS PLANO MISTO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR FONTE CUSTEIO ADM DOS INVESTIMENTOS PREVER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR LIQ CCA DA PATROC FAPERS P/ PGS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR LIQ CCA DA PATROC FAPERS P/ PREVER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR LIQ CCA PARTIC ATIVOS DA PATROC FAPERS P/ PGS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR LIQ CCA PARTIC ATIVOS DA PATROC FAPERS P/ PREVER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR LIQ CONTR PARTIC ATIVOS DA PATROC FAPERS P/ PLANO MISTO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROPR TICKET SERV S/A REF ALIMENTAÇÃO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROPR TICKET SERV S/A REF REFEIÇÃO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROPR TICKET SERV S/A REF REFEIÇÃO ESTAGIÁRIOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLR PENSAO ALIMENTICIA CFE FL PAGTO </t>
   </si>
 </sst>
 </file>
@@ -2622,7 +2619,9 @@
   </sheetPr>
   <dimension ref="A1:B298"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5029,8 +5028,8 @@
   </sheetPr>
   <dimension ref="A1:D427"/>
   <sheetViews>
-    <sheetView topLeftCell="A413" workbookViewId="0">
-      <selection activeCell="D419" sqref="D419"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5057,7 +5056,7 @@
         <v>112</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>605</v>
+        <v>627</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -5067,7 +5066,7 @@
         <v>112</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>606</v>
+        <v>628</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -5077,7 +5076,7 @@
         <v>112</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>607</v>
+        <v>629</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -5087,7 +5086,7 @@
         <v>112</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>614</v>
+        <v>580</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -5097,7 +5096,7 @@
         <v>993</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>649</v>
+        <v>612</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -5107,7 +5106,7 @@
         <v>993</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>650</v>
+        <v>613</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -5117,7 +5116,7 @@
         <v>112</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>448</v>
+        <v>630</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -5127,7 +5126,7 @@
         <v>112</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>449</v>
+        <v>631</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -5137,7 +5136,7 @@
         <v>112</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>450</v>
+        <v>632</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -5147,7 +5146,7 @@
         <v>116</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>263</v>
+        <v>633</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -5157,7 +5156,7 @@
         <v>103</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -5167,7 +5166,7 @@
         <v>103</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>634</v>
+        <v>600</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -5177,7 +5176,7 @@
         <v>103</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>451</v>
+        <v>622</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -5187,7 +5186,7 @@
         <v>103</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>454</v>
+        <v>623</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -5197,7 +5196,7 @@
         <v>103</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>455</v>
+        <v>623</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -5207,7 +5206,7 @@
         <v>518</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>481</v>
+        <v>453</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -5217,7 +5216,7 @@
         <v>518</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>651</v>
+        <v>614</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -5227,7 +5226,7 @@
         <v>518</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>652</v>
+        <v>615</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -5237,7 +5236,7 @@
         <v>518</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>484</v>
+        <v>456</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -5247,7 +5246,7 @@
         <v>518</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>653</v>
+        <v>616</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -5257,7 +5256,7 @@
         <v>201</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>654</v>
+        <v>617</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -5267,7 +5266,7 @@
         <v>201</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>655</v>
+        <v>618</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -5277,7 +5276,7 @@
         <v>201</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>656</v>
+        <v>619</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -5287,7 +5286,7 @@
         <v>103</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>657</v>
+        <v>620</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -5297,7 +5296,7 @@
         <v>103</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -5307,7 +5306,7 @@
         <v>116</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>264</v>
+        <v>634</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -5317,7 +5316,7 @@
         <v>118</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>260</v>
+        <v>655</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -5327,7 +5326,7 @@
         <v>118</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>261</v>
+        <v>656</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -5337,7 +5336,7 @@
         <v>118</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -5347,7 +5346,7 @@
         <v>110</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -5357,7 +5356,7 @@
         <v>110</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>461</v>
+        <v>438</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -5367,7 +5366,7 @@
         <v>110</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>462</v>
+        <v>439</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -5377,7 +5376,7 @@
         <v>110</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -5387,7 +5386,7 @@
         <v>110</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>466</v>
+        <v>443</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -5397,7 +5396,7 @@
         <v>110</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>467</v>
+        <v>444</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -5407,7 +5406,7 @@
         <v>110</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>468</v>
+        <v>445</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -5417,7 +5416,7 @@
         <v>110</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>469</v>
+        <v>446</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -5427,7 +5426,7 @@
         <v>110</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>465</v>
+        <v>442</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -5437,7 +5436,7 @@
         <v>110</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>470</v>
+        <v>447</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -5447,7 +5446,7 @@
         <v>103</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>474</v>
+        <v>451</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -5457,7 +5456,7 @@
         <v>101</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>568</v>
+        <v>540</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -5467,7 +5466,7 @@
         <v>103</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -5487,7 +5486,7 @@
         <v>103</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>441</v>
+        <v>635</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -5497,7 +5496,7 @@
         <v>103</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -5507,7 +5506,7 @@
         <v>103</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -5517,7 +5516,7 @@
         <v>103</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>438</v>
+        <v>658</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -5527,7 +5526,7 @@
         <v>103</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -5537,7 +5536,7 @@
         <v>103</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -5547,7 +5546,7 @@
         <v>103</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -5557,7 +5556,7 @@
         <v>106</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>255</v>
+        <v>636</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -5567,7 +5566,7 @@
         <v>106</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>253</v>
+        <v>637</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -5577,7 +5576,7 @@
         <v>106</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>254</v>
+        <v>638</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -5587,7 +5586,7 @@
         <v>106</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>256</v>
+        <v>639</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -5597,7 +5596,7 @@
         <v>108</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>245</v>
+        <v>640</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -5607,7 +5606,7 @@
         <v>109</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>602</v>
+        <v>574</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -5617,7 +5616,7 @@
         <v>110</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -5627,7 +5626,7 @@
         <v>110</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>457</v>
+        <v>434</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -5637,7 +5636,7 @@
         <v>110</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>456</v>
+        <v>433</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -5647,7 +5646,7 @@
         <v>110</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>452</v>
+        <v>431</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -5657,7 +5656,7 @@
         <v>110</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -5667,7 +5666,7 @@
         <v>110</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -5677,7 +5676,7 @@
         <v>112</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>447</v>
+        <v>641</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -5687,7 +5686,7 @@
         <v>112</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>610</v>
+        <v>642</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -5697,7 +5696,7 @@
         <v>112</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>609</v>
+        <v>643</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -5707,7 +5706,7 @@
         <v>112</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>608</v>
+        <v>644</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -5717,7 +5716,7 @@
         <v>115</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -5727,7 +5726,7 @@
         <v>116</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>262</v>
+        <v>645</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -5737,7 +5736,7 @@
         <v>116</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>265</v>
+        <v>646</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -5747,7 +5746,7 @@
         <v>124</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -5757,7 +5756,7 @@
         <v>201</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>492</v>
+        <v>464</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -5767,7 +5766,7 @@
         <v>201</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>544</v>
+        <v>516</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -5777,7 +5776,7 @@
         <v>201</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>507</v>
+        <v>479</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -5787,7 +5786,7 @@
         <v>201</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>508</v>
+        <v>480</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -5797,7 +5796,7 @@
         <v>201</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>526</v>
+        <v>498</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -5807,7 +5806,7 @@
         <v>201</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>625</v>
+        <v>591</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -5817,7 +5816,7 @@
         <v>201</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>585</v>
+        <v>557</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -5827,7 +5826,7 @@
         <v>201</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>584</v>
+        <v>556</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -5835,7 +5834,7 @@
         <v>201</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>546</v>
+        <v>518</v>
       </c>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.3">
@@ -5843,7 +5842,7 @@
         <v>201</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>604</v>
+        <v>576</v>
       </c>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.3">
@@ -5851,7 +5850,7 @@
         <v>201</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>567</v>
+        <v>539</v>
       </c>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.3">
@@ -5859,7 +5858,7 @@
         <v>201</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>570</v>
+        <v>542</v>
       </c>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.3">
@@ -5867,7 +5866,7 @@
         <v>201</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>565</v>
+        <v>537</v>
       </c>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.3">
@@ -5875,7 +5874,7 @@
         <v>201</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>583</v>
+        <v>555</v>
       </c>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.3">
@@ -5883,7 +5882,7 @@
         <v>201</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>509</v>
+        <v>481</v>
       </c>
     </row>
     <row r="87" spans="3:4" x14ac:dyDescent="0.3">
@@ -5891,7 +5890,7 @@
         <v>201</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
     </row>
     <row r="88" spans="3:4" x14ac:dyDescent="0.3">
@@ -5899,7 +5898,7 @@
         <v>201</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>637</v>
+        <v>603</v>
       </c>
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.3">
@@ -5907,7 +5906,7 @@
         <v>201</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>632</v>
+        <v>598</v>
       </c>
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.3">
@@ -5915,7 +5914,7 @@
         <v>201</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>523</v>
+        <v>495</v>
       </c>
     </row>
     <row r="91" spans="3:4" x14ac:dyDescent="0.3">
@@ -5923,7 +5922,7 @@
         <v>201</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>547</v>
+        <v>519</v>
       </c>
     </row>
     <row r="92" spans="3:4" x14ac:dyDescent="0.3">
@@ -5931,7 +5930,7 @@
         <v>201</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>510</v>
+        <v>482</v>
       </c>
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.3">
@@ -5939,7 +5938,7 @@
         <v>201</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>592</v>
+        <v>564</v>
       </c>
     </row>
     <row r="94" spans="3:4" x14ac:dyDescent="0.3">
@@ -5947,7 +5946,7 @@
         <v>201</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>524</v>
+        <v>496</v>
       </c>
     </row>
     <row r="95" spans="3:4" x14ac:dyDescent="0.3">
@@ -5955,7 +5954,7 @@
         <v>201</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="96" spans="3:4" x14ac:dyDescent="0.3">
@@ -5963,7 +5962,7 @@
         <v>201</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>594</v>
+        <v>566</v>
       </c>
     </row>
     <row r="97" spans="3:4" x14ac:dyDescent="0.3">
@@ -5971,7 +5970,7 @@
         <v>201</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="98" spans="3:4" x14ac:dyDescent="0.3">
@@ -5979,7 +5978,7 @@
         <v>201</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>595</v>
+        <v>567</v>
       </c>
     </row>
     <row r="99" spans="3:4" x14ac:dyDescent="0.3">
@@ -5995,7 +5994,7 @@
         <v>201</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>548</v>
+        <v>520</v>
       </c>
     </row>
     <row r="101" spans="3:4" x14ac:dyDescent="0.3">
@@ -6003,7 +6002,7 @@
         <v>201</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>562</v>
+        <v>534</v>
       </c>
     </row>
     <row r="102" spans="3:4" x14ac:dyDescent="0.3">
@@ -6011,7 +6010,7 @@
         <v>201</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>473</v>
+        <v>450</v>
       </c>
     </row>
     <row r="103" spans="3:4" x14ac:dyDescent="0.3">
@@ -6019,7 +6018,7 @@
         <v>201</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>556</v>
+        <v>528</v>
       </c>
     </row>
     <row r="104" spans="3:4" x14ac:dyDescent="0.3">
@@ -6027,7 +6026,7 @@
         <v>201</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>540</v>
+        <v>512</v>
       </c>
     </row>
     <row r="105" spans="3:4" x14ac:dyDescent="0.3">
@@ -6035,7 +6034,7 @@
         <v>201</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>515</v>
+        <v>487</v>
       </c>
     </row>
     <row r="106" spans="3:4" x14ac:dyDescent="0.3">
@@ -6043,7 +6042,7 @@
         <v>201</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>635</v>
+        <v>601</v>
       </c>
     </row>
     <row r="107" spans="3:4" x14ac:dyDescent="0.3">
@@ -6051,7 +6050,7 @@
         <v>201</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>627</v>
+        <v>593</v>
       </c>
     </row>
     <row r="108" spans="3:4" x14ac:dyDescent="0.3">
@@ -6059,7 +6058,7 @@
         <v>201</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>538</v>
+        <v>510</v>
       </c>
     </row>
     <row r="109" spans="3:4" x14ac:dyDescent="0.3">
@@ -6067,7 +6066,7 @@
         <v>201</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>516</v>
+        <v>488</v>
       </c>
     </row>
     <row r="110" spans="3:4" x14ac:dyDescent="0.3">
@@ -6075,7 +6074,7 @@
         <v>201</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>636</v>
+        <v>602</v>
       </c>
     </row>
     <row r="111" spans="3:4" x14ac:dyDescent="0.3">
@@ -6083,7 +6082,7 @@
         <v>201</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>628</v>
+        <v>594</v>
       </c>
     </row>
     <row r="112" spans="3:4" x14ac:dyDescent="0.3">
@@ -6091,7 +6090,7 @@
         <v>201</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>494</v>
+        <v>466</v>
       </c>
     </row>
     <row r="113" spans="3:4" x14ac:dyDescent="0.3">
@@ -6099,7 +6098,7 @@
         <v>201</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>616</v>
+        <v>582</v>
       </c>
     </row>
     <row r="114" spans="3:4" x14ac:dyDescent="0.3">
@@ -6107,7 +6106,7 @@
         <v>201</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>617</v>
+        <v>583</v>
       </c>
     </row>
     <row r="115" spans="3:4" x14ac:dyDescent="0.3">
@@ -6115,7 +6114,7 @@
         <v>201</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>615</v>
+        <v>581</v>
       </c>
     </row>
     <row r="116" spans="3:4" x14ac:dyDescent="0.3">
@@ -6123,7 +6122,7 @@
         <v>201</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="117" spans="3:4" x14ac:dyDescent="0.3">
@@ -6131,7 +6130,7 @@
         <v>201</v>
       </c>
       <c r="D117" s="9" t="s">
-        <v>528</v>
+        <v>500</v>
       </c>
     </row>
     <row r="118" spans="3:4" x14ac:dyDescent="0.3">
@@ -6139,7 +6138,7 @@
         <v>201</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="119" spans="3:4" x14ac:dyDescent="0.3">
@@ -6147,7 +6146,7 @@
         <v>201</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>530</v>
+        <v>502</v>
       </c>
     </row>
     <row r="120" spans="3:4" x14ac:dyDescent="0.3">
@@ -6155,7 +6154,7 @@
         <v>201</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>529</v>
+        <v>501</v>
       </c>
     </row>
     <row r="121" spans="3:4" x14ac:dyDescent="0.3">
@@ -6163,7 +6162,7 @@
         <v>201</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="122" spans="3:4" x14ac:dyDescent="0.3">
@@ -6171,7 +6170,7 @@
         <v>201</v>
       </c>
       <c r="D122" s="9" t="s">
-        <v>532</v>
+        <v>504</v>
       </c>
     </row>
     <row r="123" spans="3:4" x14ac:dyDescent="0.3">
@@ -6179,7 +6178,7 @@
         <v>201</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>531</v>
+        <v>503</v>
       </c>
     </row>
     <row r="124" spans="3:4" x14ac:dyDescent="0.3">
@@ -6187,7 +6186,7 @@
         <v>201</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>618</v>
+        <v>584</v>
       </c>
     </row>
     <row r="125" spans="3:4" x14ac:dyDescent="0.3">
@@ -6195,7 +6194,7 @@
         <v>201</v>
       </c>
       <c r="D125" s="9" t="s">
-        <v>619</v>
+        <v>585</v>
       </c>
     </row>
     <row r="126" spans="3:4" x14ac:dyDescent="0.3">
@@ -6203,7 +6202,7 @@
         <v>201</v>
       </c>
       <c r="D126" s="9" t="s">
-        <v>558</v>
+        <v>530</v>
       </c>
     </row>
     <row r="127" spans="3:4" x14ac:dyDescent="0.3">
@@ -6211,7 +6210,7 @@
         <v>201</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>578</v>
+        <v>550</v>
       </c>
     </row>
     <row r="128" spans="3:4" x14ac:dyDescent="0.3">
@@ -6219,7 +6218,7 @@
         <v>201</v>
       </c>
       <c r="D128" s="9" t="s">
-        <v>504</v>
+        <v>476</v>
       </c>
     </row>
     <row r="129" spans="3:4" x14ac:dyDescent="0.3">
@@ -6227,7 +6226,7 @@
         <v>201</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>639</v>
+        <v>605</v>
       </c>
     </row>
     <row r="130" spans="3:4" x14ac:dyDescent="0.3">
@@ -6235,7 +6234,7 @@
         <v>201</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>491</v>
+        <v>463</v>
       </c>
     </row>
     <row r="131" spans="3:4" x14ac:dyDescent="0.3">
@@ -6243,7 +6242,7 @@
         <v>201</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>640</v>
+        <v>606</v>
       </c>
     </row>
     <row r="132" spans="3:4" x14ac:dyDescent="0.3">
@@ -6251,7 +6250,7 @@
         <v>201</v>
       </c>
       <c r="D132" s="9" t="s">
-        <v>505</v>
+        <v>477</v>
       </c>
     </row>
     <row r="133" spans="3:4" x14ac:dyDescent="0.3">
@@ -6259,7 +6258,7 @@
         <v>201</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>589</v>
+        <v>561</v>
       </c>
     </row>
     <row r="134" spans="3:4" x14ac:dyDescent="0.3">
@@ -6267,7 +6266,7 @@
         <v>201</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>590</v>
+        <v>562</v>
       </c>
     </row>
     <row r="135" spans="3:4" x14ac:dyDescent="0.3">
@@ -6275,7 +6274,7 @@
         <v>201</v>
       </c>
       <c r="D135" s="9" t="s">
-        <v>591</v>
+        <v>563</v>
       </c>
     </row>
     <row r="136" spans="3:4" x14ac:dyDescent="0.3">
@@ -6283,7 +6282,7 @@
         <v>201</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>513</v>
+        <v>485</v>
       </c>
     </row>
     <row r="137" spans="3:4" x14ac:dyDescent="0.3">
@@ -6291,7 +6290,7 @@
         <v>201</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>488</v>
+        <v>460</v>
       </c>
     </row>
     <row r="138" spans="3:4" x14ac:dyDescent="0.3">
@@ -6299,7 +6298,7 @@
         <v>201</v>
       </c>
       <c r="D138" s="9" t="s">
-        <v>641</v>
+        <v>607</v>
       </c>
     </row>
     <row r="139" spans="3:4" x14ac:dyDescent="0.3">
@@ -6307,7 +6306,7 @@
         <v>201</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>520</v>
+        <v>492</v>
       </c>
     </row>
     <row r="140" spans="3:4" x14ac:dyDescent="0.3">
@@ -6315,7 +6314,7 @@
         <v>201</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>642</v>
+        <v>608</v>
       </c>
     </row>
     <row r="141" spans="3:4" x14ac:dyDescent="0.3">
@@ -6323,7 +6322,7 @@
         <v>201</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="142" spans="3:4" x14ac:dyDescent="0.3">
@@ -6331,7 +6330,7 @@
         <v>201</v>
       </c>
       <c r="D142" s="9" t="s">
-        <v>514</v>
+        <v>486</v>
       </c>
     </row>
     <row r="143" spans="3:4" x14ac:dyDescent="0.3">
@@ -6339,7 +6338,7 @@
         <v>201</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>643</v>
+        <v>609</v>
       </c>
     </row>
     <row r="144" spans="3:4" x14ac:dyDescent="0.3">
@@ -6347,7 +6346,7 @@
         <v>201</v>
       </c>
       <c r="D144" s="9" t="s">
-        <v>550</v>
+        <v>522</v>
       </c>
     </row>
     <row r="145" spans="3:4" x14ac:dyDescent="0.3">
@@ -6355,7 +6354,7 @@
         <v>201</v>
       </c>
       <c r="D145" s="9" t="s">
-        <v>551</v>
+        <v>523</v>
       </c>
     </row>
     <row r="146" spans="3:4" x14ac:dyDescent="0.3">
@@ -6363,7 +6362,7 @@
         <v>201</v>
       </c>
       <c r="D146" s="9" t="s">
-        <v>593</v>
+        <v>565</v>
       </c>
     </row>
     <row r="147" spans="3:4" x14ac:dyDescent="0.3">
@@ -6371,7 +6370,7 @@
         <v>201</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>561</v>
+        <v>533</v>
       </c>
     </row>
     <row r="148" spans="3:4" x14ac:dyDescent="0.3">
@@ -6379,7 +6378,7 @@
         <v>201</v>
       </c>
       <c r="D148" s="9" t="s">
-        <v>572</v>
+        <v>544</v>
       </c>
     </row>
     <row r="149" spans="3:4" x14ac:dyDescent="0.3">
@@ -6387,7 +6386,7 @@
         <v>201</v>
       </c>
       <c r="D149" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="150" spans="3:4" x14ac:dyDescent="0.3">
@@ -6395,7 +6394,7 @@
         <v>201</v>
       </c>
       <c r="D150" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="151" spans="3:4" x14ac:dyDescent="0.3">
@@ -6403,7 +6402,7 @@
         <v>202</v>
       </c>
       <c r="D151" s="9" t="s">
-        <v>493</v>
+        <v>465</v>
       </c>
     </row>
     <row r="152" spans="3:4" x14ac:dyDescent="0.3">
@@ -6411,7 +6410,7 @@
         <v>202</v>
       </c>
       <c r="D152" s="9" t="s">
-        <v>545</v>
+        <v>517</v>
       </c>
     </row>
     <row r="153" spans="3:4" x14ac:dyDescent="0.3">
@@ -6419,7 +6418,7 @@
         <v>202</v>
       </c>
       <c r="D153" s="9" t="s">
-        <v>648</v>
+        <v>611</v>
       </c>
     </row>
     <row r="154" spans="3:4" x14ac:dyDescent="0.3">
@@ -6427,7 +6426,7 @@
         <v>202</v>
       </c>
       <c r="D154" s="9" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
     </row>
     <row r="155" spans="3:4" x14ac:dyDescent="0.3">
@@ -6435,7 +6434,7 @@
         <v>202</v>
       </c>
       <c r="D155" s="9" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
     </row>
     <row r="156" spans="3:4" x14ac:dyDescent="0.3">
@@ -6443,7 +6442,7 @@
         <v>202</v>
       </c>
       <c r="D156" s="9" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
     </row>
     <row r="157" spans="3:4" x14ac:dyDescent="0.3">
@@ -6451,7 +6450,7 @@
         <v>202</v>
       </c>
       <c r="D157" s="9" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
     </row>
     <row r="158" spans="3:4" x14ac:dyDescent="0.3">
@@ -6459,7 +6458,7 @@
         <v>202</v>
       </c>
       <c r="D158" s="9" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
     </row>
     <row r="159" spans="3:4" x14ac:dyDescent="0.3">
@@ -6467,7 +6466,7 @@
         <v>202</v>
       </c>
       <c r="D159" s="9" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
     </row>
     <row r="160" spans="3:4" x14ac:dyDescent="0.3">
@@ -6475,7 +6474,7 @@
         <v>202</v>
       </c>
       <c r="D160" s="9" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
     </row>
     <row r="161" spans="3:4" x14ac:dyDescent="0.3">
@@ -6483,7 +6482,7 @@
         <v>202</v>
       </c>
       <c r="D161" s="9" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
     </row>
     <row r="162" spans="3:4" x14ac:dyDescent="0.3">
@@ -6491,7 +6490,7 @@
         <v>202</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
     </row>
     <row r="163" spans="3:4" x14ac:dyDescent="0.3">
@@ -6499,7 +6498,7 @@
         <v>202</v>
       </c>
       <c r="D163" s="9" t="s">
-        <v>613</v>
+        <v>579</v>
       </c>
     </row>
     <row r="164" spans="3:4" x14ac:dyDescent="0.3">
@@ -6507,7 +6506,7 @@
         <v>202</v>
       </c>
       <c r="D164" s="9" t="s">
-        <v>612</v>
+        <v>578</v>
       </c>
     </row>
     <row r="165" spans="3:4" x14ac:dyDescent="0.3">
@@ -6515,7 +6514,7 @@
         <v>202</v>
       </c>
       <c r="D165" s="9" t="s">
-        <v>611</v>
+        <v>577</v>
       </c>
     </row>
     <row r="166" spans="3:4" x14ac:dyDescent="0.3">
@@ -6523,7 +6522,7 @@
         <v>202</v>
       </c>
       <c r="D166" s="9" t="s">
-        <v>459</v>
+        <v>436</v>
       </c>
     </row>
     <row r="167" spans="3:4" x14ac:dyDescent="0.3">
@@ -6603,7 +6602,7 @@
         <v>202</v>
       </c>
       <c r="D176" s="9" t="s">
-        <v>525</v>
+        <v>497</v>
       </c>
     </row>
     <row r="177" spans="3:4" x14ac:dyDescent="0.3">
@@ -6611,7 +6610,7 @@
         <v>202</v>
       </c>
       <c r="D177" s="9" t="s">
-        <v>626</v>
+        <v>592</v>
       </c>
     </row>
     <row r="178" spans="3:4" x14ac:dyDescent="0.3">
@@ -6619,7 +6618,7 @@
         <v>202</v>
       </c>
       <c r="D178" s="9" t="s">
-        <v>587</v>
+        <v>559</v>
       </c>
     </row>
     <row r="179" spans="3:4" x14ac:dyDescent="0.3">
@@ -6627,7 +6626,7 @@
         <v>202</v>
       </c>
       <c r="D179" s="9" t="s">
-        <v>588</v>
+        <v>560</v>
       </c>
     </row>
     <row r="180" spans="3:4" x14ac:dyDescent="0.3">
@@ -6635,7 +6634,7 @@
         <v>202</v>
       </c>
       <c r="D180" s="9" t="s">
-        <v>596</v>
+        <v>568</v>
       </c>
     </row>
     <row r="181" spans="3:4" x14ac:dyDescent="0.3">
@@ -6643,7 +6642,7 @@
         <v>202</v>
       </c>
       <c r="D181" s="9" t="s">
-        <v>597</v>
+        <v>569</v>
       </c>
     </row>
     <row r="182" spans="3:4" x14ac:dyDescent="0.3">
@@ -6651,7 +6650,7 @@
         <v>202</v>
       </c>
       <c r="D182" s="9" t="s">
-        <v>549</v>
+        <v>521</v>
       </c>
     </row>
     <row r="183" spans="3:4" x14ac:dyDescent="0.3">
@@ -6659,7 +6658,7 @@
         <v>202</v>
       </c>
       <c r="D183" s="9" t="s">
-        <v>564</v>
+        <v>536</v>
       </c>
     </row>
     <row r="184" spans="3:4" x14ac:dyDescent="0.3">
@@ -6667,7 +6666,7 @@
         <v>202</v>
       </c>
       <c r="D184" s="9" t="s">
-        <v>575</v>
+        <v>547</v>
       </c>
     </row>
     <row r="185" spans="3:4" x14ac:dyDescent="0.3">
@@ -6675,7 +6674,7 @@
         <v>202</v>
       </c>
       <c r="D185" s="9" t="s">
-        <v>574</v>
+        <v>546</v>
       </c>
     </row>
     <row r="186" spans="3:4" x14ac:dyDescent="0.3">
@@ -6683,7 +6682,7 @@
         <v>202</v>
       </c>
       <c r="D186" s="9" t="s">
-        <v>571</v>
+        <v>543</v>
       </c>
     </row>
     <row r="187" spans="3:4" x14ac:dyDescent="0.3">
@@ -6691,7 +6690,7 @@
         <v>202</v>
       </c>
       <c r="D187" s="9" t="s">
-        <v>576</v>
+        <v>548</v>
       </c>
     </row>
     <row r="188" spans="3:4" x14ac:dyDescent="0.3">
@@ -6699,7 +6698,7 @@
         <v>202</v>
       </c>
       <c r="D188" s="9" t="s">
-        <v>495</v>
+        <v>467</v>
       </c>
     </row>
     <row r="189" spans="3:4" x14ac:dyDescent="0.3">
@@ -6707,7 +6706,7 @@
         <v>202</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>552</v>
+        <v>524</v>
       </c>
     </row>
     <row r="190" spans="3:4" x14ac:dyDescent="0.3">
@@ -6715,7 +6714,7 @@
         <v>202</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>496</v>
+        <v>468</v>
       </c>
     </row>
     <row r="191" spans="3:4" x14ac:dyDescent="0.3">
@@ -6723,7 +6722,7 @@
         <v>202</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>579</v>
+        <v>551</v>
       </c>
     </row>
     <row r="192" spans="3:4" x14ac:dyDescent="0.3">
@@ -6731,7 +6730,7 @@
         <v>202</v>
       </c>
       <c r="D192" s="9" t="s">
-        <v>553</v>
+        <v>525</v>
       </c>
     </row>
     <row r="193" spans="3:4" x14ac:dyDescent="0.3">
@@ -6739,7 +6738,7 @@
         <v>202</v>
       </c>
       <c r="D193" s="9" t="s">
-        <v>554</v>
+        <v>526</v>
       </c>
     </row>
     <row r="194" spans="3:4" x14ac:dyDescent="0.3">
@@ -6747,7 +6746,7 @@
         <v>202</v>
       </c>
       <c r="D194" s="9" t="s">
-        <v>555</v>
+        <v>527</v>
       </c>
     </row>
     <row r="195" spans="3:4" x14ac:dyDescent="0.3">
@@ -6755,7 +6754,7 @@
         <v>202</v>
       </c>
       <c r="D195" s="9" t="s">
-        <v>603</v>
+        <v>575</v>
       </c>
     </row>
     <row r="196" spans="3:4" x14ac:dyDescent="0.3">
@@ -6763,7 +6762,7 @@
         <v>202</v>
       </c>
       <c r="D196" s="9" t="s">
-        <v>527</v>
+        <v>499</v>
       </c>
     </row>
     <row r="197" spans="3:4" x14ac:dyDescent="0.3">
@@ -6771,7 +6770,7 @@
         <v>202</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>580</v>
+        <v>552</v>
       </c>
     </row>
     <row r="198" spans="3:4" x14ac:dyDescent="0.3">
@@ -6779,7 +6778,7 @@
         <v>202</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>581</v>
+        <v>553</v>
       </c>
     </row>
     <row r="199" spans="3:4" x14ac:dyDescent="0.3">
@@ -6787,7 +6786,7 @@
         <v>202</v>
       </c>
       <c r="D199" s="9" t="s">
-        <v>497</v>
+        <v>469</v>
       </c>
     </row>
     <row r="200" spans="3:4" x14ac:dyDescent="0.3">
@@ -6795,7 +6794,7 @@
         <v>202</v>
       </c>
       <c r="D200" s="9" t="s">
-        <v>541</v>
+        <v>513</v>
       </c>
     </row>
     <row r="201" spans="3:4" x14ac:dyDescent="0.3">
@@ -6803,7 +6802,7 @@
         <v>202</v>
       </c>
       <c r="D201" s="9" t="s">
-        <v>489</v>
+        <v>461</v>
       </c>
     </row>
     <row r="202" spans="3:4" x14ac:dyDescent="0.3">
@@ -6811,7 +6810,7 @@
         <v>202</v>
       </c>
       <c r="D202" s="9" t="s">
-        <v>560</v>
+        <v>532</v>
       </c>
     </row>
     <row r="203" spans="3:4" x14ac:dyDescent="0.3">
@@ -6819,7 +6818,7 @@
         <v>202</v>
       </c>
       <c r="D203" s="9" t="s">
-        <v>517</v>
+        <v>489</v>
       </c>
     </row>
     <row r="204" spans="3:4" x14ac:dyDescent="0.3">
@@ -6827,7 +6826,7 @@
         <v>202</v>
       </c>
       <c r="D204" s="9" t="s">
-        <v>542</v>
+        <v>514</v>
       </c>
     </row>
     <row r="205" spans="3:4" x14ac:dyDescent="0.3">
@@ -6835,7 +6834,7 @@
         <v>202</v>
       </c>
       <c r="D205" s="9" t="s">
-        <v>557</v>
+        <v>529</v>
       </c>
     </row>
     <row r="206" spans="3:4" x14ac:dyDescent="0.3">
@@ -6843,7 +6842,7 @@
         <v>202</v>
       </c>
       <c r="D206" s="9" t="s">
-        <v>543</v>
+        <v>515</v>
       </c>
     </row>
     <row r="207" spans="3:4" x14ac:dyDescent="0.3">
@@ -6851,7 +6850,7 @@
         <v>202</v>
       </c>
       <c r="D207" s="9" t="s">
-        <v>453</v>
+        <v>432</v>
       </c>
     </row>
     <row r="208" spans="3:4" x14ac:dyDescent="0.3">
@@ -6859,7 +6858,7 @@
         <v>202</v>
       </c>
       <c r="D208" s="9" t="s">
-        <v>633</v>
+        <v>599</v>
       </c>
     </row>
     <row r="209" spans="3:4" x14ac:dyDescent="0.3">
@@ -6867,7 +6866,7 @@
         <v>202</v>
       </c>
       <c r="D209" s="9" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
     </row>
     <row r="210" spans="3:4" x14ac:dyDescent="0.3">
@@ -6875,7 +6874,7 @@
         <v>202</v>
       </c>
       <c r="D210" s="9" t="s">
-        <v>471</v>
+        <v>448</v>
       </c>
     </row>
     <row r="211" spans="3:4" x14ac:dyDescent="0.3">
@@ -6883,7 +6882,7 @@
         <v>202</v>
       </c>
       <c r="D211" s="9" t="s">
-        <v>472</v>
+        <v>449</v>
       </c>
     </row>
     <row r="212" spans="3:4" x14ac:dyDescent="0.3">
@@ -6891,7 +6890,7 @@
         <v>202</v>
       </c>
       <c r="D212" s="9" t="s">
-        <v>499</v>
+        <v>471</v>
       </c>
     </row>
     <row r="213" spans="3:4" x14ac:dyDescent="0.3">
@@ -6899,7 +6898,7 @@
         <v>202</v>
       </c>
       <c r="D213" s="9" t="s">
-        <v>503</v>
+        <v>475</v>
       </c>
     </row>
     <row r="214" spans="3:4" x14ac:dyDescent="0.3">
@@ -6907,7 +6906,7 @@
         <v>202</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>566</v>
+        <v>538</v>
       </c>
     </row>
     <row r="215" spans="3:4" x14ac:dyDescent="0.3">
@@ -6915,7 +6914,7 @@
         <v>202</v>
       </c>
       <c r="D215" s="9" t="s">
-        <v>518</v>
+        <v>490</v>
       </c>
     </row>
     <row r="216" spans="3:4" x14ac:dyDescent="0.3">
@@ -6923,7 +6922,7 @@
         <v>202</v>
       </c>
       <c r="D216" s="9" t="s">
-        <v>521</v>
+        <v>493</v>
       </c>
     </row>
     <row r="217" spans="3:4" x14ac:dyDescent="0.3">
@@ -6931,7 +6930,7 @@
         <v>202</v>
       </c>
       <c r="D217" s="9" t="s">
-        <v>539</v>
+        <v>511</v>
       </c>
     </row>
     <row r="218" spans="3:4" x14ac:dyDescent="0.3">
@@ -6939,7 +6938,7 @@
         <v>202</v>
       </c>
       <c r="D218" s="9" t="s">
-        <v>511</v>
+        <v>483</v>
       </c>
     </row>
     <row r="219" spans="3:4" x14ac:dyDescent="0.3">
@@ -6947,7 +6946,7 @@
         <v>202</v>
       </c>
       <c r="D219" s="9" t="s">
-        <v>486</v>
+        <v>458</v>
       </c>
     </row>
     <row r="220" spans="3:4" x14ac:dyDescent="0.3">
@@ -6955,7 +6954,7 @@
         <v>202</v>
       </c>
       <c r="D220" s="9" t="s">
-        <v>519</v>
+        <v>491</v>
       </c>
     </row>
     <row r="221" spans="3:4" x14ac:dyDescent="0.3">
@@ -6963,7 +6962,7 @@
         <v>202</v>
       </c>
       <c r="D221" s="9" t="s">
-        <v>498</v>
+        <v>470</v>
       </c>
     </row>
     <row r="222" spans="3:4" x14ac:dyDescent="0.3">
@@ -6971,7 +6970,7 @@
         <v>202</v>
       </c>
       <c r="D222" s="9" t="s">
-        <v>582</v>
+        <v>554</v>
       </c>
     </row>
     <row r="223" spans="3:4" x14ac:dyDescent="0.3">
@@ -6979,7 +6978,7 @@
         <v>202</v>
       </c>
       <c r="D223" s="9" t="s">
-        <v>512</v>
+        <v>484</v>
       </c>
     </row>
     <row r="224" spans="3:4" x14ac:dyDescent="0.3">
@@ -6987,7 +6986,7 @@
         <v>202</v>
       </c>
       <c r="D224" s="9" t="s">
-        <v>500</v>
+        <v>472</v>
       </c>
     </row>
     <row r="225" spans="3:4" x14ac:dyDescent="0.3">
@@ -6995,7 +6994,7 @@
         <v>202</v>
       </c>
       <c r="D225" s="9" t="s">
-        <v>620</v>
+        <v>586</v>
       </c>
     </row>
     <row r="226" spans="3:4" x14ac:dyDescent="0.3">
@@ -7003,7 +7002,7 @@
         <v>202</v>
       </c>
       <c r="D226" s="9" t="s">
-        <v>621</v>
+        <v>587</v>
       </c>
     </row>
     <row r="227" spans="3:4" x14ac:dyDescent="0.3">
@@ -7011,7 +7010,7 @@
         <v>202</v>
       </c>
       <c r="D227" s="9" t="s">
-        <v>622</v>
+        <v>588</v>
       </c>
     </row>
     <row r="228" spans="3:4" x14ac:dyDescent="0.3">
@@ -7019,7 +7018,7 @@
         <v>202</v>
       </c>
       <c r="D228" s="9" t="s">
-        <v>533</v>
+        <v>505</v>
       </c>
     </row>
     <row r="229" spans="3:4" x14ac:dyDescent="0.3">
@@ -7027,7 +7026,7 @@
         <v>202</v>
       </c>
       <c r="D229" s="9" t="s">
-        <v>535</v>
+        <v>507</v>
       </c>
     </row>
     <row r="230" spans="3:4" x14ac:dyDescent="0.3">
@@ -7035,7 +7034,7 @@
         <v>202</v>
       </c>
       <c r="D230" s="9" t="s">
-        <v>534</v>
+        <v>506</v>
       </c>
     </row>
     <row r="231" spans="3:4" x14ac:dyDescent="0.3">
@@ -7043,7 +7042,7 @@
         <v>202</v>
       </c>
       <c r="D231" s="9" t="s">
-        <v>537</v>
+        <v>509</v>
       </c>
     </row>
     <row r="232" spans="3:4" x14ac:dyDescent="0.3">
@@ -7051,7 +7050,7 @@
         <v>202</v>
       </c>
       <c r="D232" s="9" t="s">
-        <v>536</v>
+        <v>508</v>
       </c>
     </row>
     <row r="233" spans="3:4" x14ac:dyDescent="0.3">
@@ -7059,7 +7058,7 @@
         <v>202</v>
       </c>
       <c r="D233" s="9" t="s">
-        <v>623</v>
+        <v>589</v>
       </c>
     </row>
     <row r="234" spans="3:4" x14ac:dyDescent="0.3">
@@ -7067,7 +7066,7 @@
         <v>202</v>
       </c>
       <c r="D234" s="9" t="s">
-        <v>624</v>
+        <v>590</v>
       </c>
     </row>
     <row r="235" spans="3:4" x14ac:dyDescent="0.3">
@@ -7075,7 +7074,7 @@
         <v>202</v>
       </c>
       <c r="D235" s="9" t="s">
-        <v>559</v>
+        <v>531</v>
       </c>
     </row>
     <row r="236" spans="3:4" x14ac:dyDescent="0.3">
@@ -7083,7 +7082,7 @@
         <v>202</v>
       </c>
       <c r="D236" s="9" t="s">
-        <v>586</v>
+        <v>558</v>
       </c>
     </row>
     <row r="237" spans="3:4" x14ac:dyDescent="0.3">
@@ -7091,7 +7090,7 @@
         <v>202</v>
       </c>
       <c r="D237" s="9" t="s">
-        <v>569</v>
+        <v>541</v>
       </c>
     </row>
     <row r="238" spans="3:4" x14ac:dyDescent="0.3">
@@ -7099,7 +7098,7 @@
         <v>202</v>
       </c>
       <c r="D238" s="9" t="s">
-        <v>563</v>
+        <v>535</v>
       </c>
     </row>
     <row r="239" spans="3:4" x14ac:dyDescent="0.3">
@@ -7107,7 +7106,7 @@
         <v>202</v>
       </c>
       <c r="D239" s="9" t="s">
-        <v>573</v>
+        <v>545</v>
       </c>
     </row>
     <row r="240" spans="3:4" x14ac:dyDescent="0.3">
@@ -7115,7 +7114,7 @@
         <v>202</v>
       </c>
       <c r="D240" s="9" t="s">
-        <v>631</v>
+        <v>597</v>
       </c>
     </row>
     <row r="241" spans="3:4" x14ac:dyDescent="0.3">
@@ -7123,7 +7122,7 @@
         <v>202</v>
       </c>
       <c r="D241" s="9" t="s">
-        <v>630</v>
+        <v>596</v>
       </c>
     </row>
     <row r="242" spans="3:4" x14ac:dyDescent="0.3">
@@ -7131,7 +7130,7 @@
         <v>202</v>
       </c>
       <c r="D242" s="9" t="s">
-        <v>638</v>
+        <v>604</v>
       </c>
     </row>
     <row r="243" spans="3:4" x14ac:dyDescent="0.3">
@@ -7139,7 +7138,7 @@
         <v>202</v>
       </c>
       <c r="D243" s="9" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
     </row>
     <row r="244" spans="3:4" x14ac:dyDescent="0.3">
@@ -7147,7 +7146,7 @@
         <v>202</v>
       </c>
       <c r="D244" s="9" t="s">
-        <v>522</v>
+        <v>494</v>
       </c>
     </row>
     <row r="245" spans="3:4" x14ac:dyDescent="0.3">
@@ -7155,7 +7154,7 @@
         <v>204</v>
       </c>
       <c r="D245" s="9" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
     </row>
     <row r="246" spans="3:4" x14ac:dyDescent="0.3">
@@ -7163,7 +7162,7 @@
         <v>204</v>
       </c>
       <c r="D246" s="9" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
     </row>
     <row r="247" spans="3:4" x14ac:dyDescent="0.3">
@@ -7171,7 +7170,7 @@
         <v>204</v>
       </c>
       <c r="D247" s="9" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
     </row>
     <row r="248" spans="3:4" x14ac:dyDescent="0.3">
@@ -7179,7 +7178,7 @@
         <v>208</v>
       </c>
       <c r="D248" s="9" t="s">
-        <v>522</v>
+        <v>494</v>
       </c>
     </row>
     <row r="249" spans="3:4" x14ac:dyDescent="0.3">
@@ -7187,7 +7186,7 @@
         <v>210</v>
       </c>
       <c r="D249" s="9" t="s">
-        <v>629</v>
+        <v>595</v>
       </c>
     </row>
     <row r="250" spans="3:4" x14ac:dyDescent="0.3">
@@ -7195,7 +7194,7 @@
         <v>210</v>
       </c>
       <c r="D250" s="9" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
     </row>
     <row r="251" spans="3:4" x14ac:dyDescent="0.3">
@@ -7203,7 +7202,7 @@
         <v>212</v>
       </c>
       <c r="D251" s="9" t="s">
-        <v>490</v>
+        <v>462</v>
       </c>
     </row>
     <row r="252" spans="3:4" x14ac:dyDescent="0.3">
@@ -7211,7 +7210,7 @@
         <v>224</v>
       </c>
       <c r="D252" s="9" t="s">
-        <v>501</v>
+        <v>473</v>
       </c>
     </row>
     <row r="253" spans="3:4" x14ac:dyDescent="0.3">
@@ -7219,7 +7218,7 @@
         <v>227</v>
       </c>
       <c r="D253" s="9" t="s">
-        <v>502</v>
+        <v>474</v>
       </c>
     </row>
     <row r="254" spans="3:4" x14ac:dyDescent="0.3">
@@ -7227,7 +7226,7 @@
         <v>400</v>
       </c>
       <c r="D254" s="9" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
     </row>
     <row r="255" spans="3:4" x14ac:dyDescent="0.3">
@@ -7235,7 +7234,7 @@
         <v>400</v>
       </c>
       <c r="D255" s="9" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
     </row>
     <row r="256" spans="3:4" x14ac:dyDescent="0.3">
@@ -7243,7 +7242,7 @@
         <v>400</v>
       </c>
       <c r="D256" s="9" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
     </row>
     <row r="257" spans="3:4" x14ac:dyDescent="0.3">
@@ -7251,7 +7250,7 @@
         <v>400</v>
       </c>
       <c r="D257" s="9" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="258" spans="3:4" x14ac:dyDescent="0.3">
@@ -7259,7 +7258,7 @@
         <v>400</v>
       </c>
       <c r="D258" s="9" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="259" spans="3:4" x14ac:dyDescent="0.3">
@@ -7267,7 +7266,7 @@
         <v>400</v>
       </c>
       <c r="D259" s="9" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
     </row>
     <row r="260" spans="3:4" x14ac:dyDescent="0.3">
@@ -7275,7 +7274,7 @@
         <v>400</v>
       </c>
       <c r="D260" s="9" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
     </row>
     <row r="261" spans="3:4" x14ac:dyDescent="0.3">
@@ -7283,7 +7282,7 @@
         <v>400</v>
       </c>
       <c r="D261" s="9" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="262" spans="3:4" x14ac:dyDescent="0.3">
@@ -7291,7 +7290,7 @@
         <v>400</v>
       </c>
       <c r="D262" s="9" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="263" spans="3:4" x14ac:dyDescent="0.3">
@@ -7299,7 +7298,7 @@
         <v>400</v>
       </c>
       <c r="D263" s="9" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
     </row>
     <row r="264" spans="3:4" x14ac:dyDescent="0.3">
@@ -7307,7 +7306,7 @@
         <v>400</v>
       </c>
       <c r="D264" s="9" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
     </row>
     <row r="265" spans="3:4" x14ac:dyDescent="0.3">
@@ -7315,7 +7314,7 @@
         <v>400</v>
       </c>
       <c r="D265" s="9" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
     </row>
     <row r="266" spans="3:4" x14ac:dyDescent="0.3">
@@ -7323,7 +7322,7 @@
         <v>400</v>
       </c>
       <c r="D266" s="9" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
     </row>
     <row r="267" spans="3:4" x14ac:dyDescent="0.3">
@@ -7331,7 +7330,7 @@
         <v>400</v>
       </c>
       <c r="D267" s="9" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
     </row>
     <row r="268" spans="3:4" x14ac:dyDescent="0.3">
@@ -7339,7 +7338,7 @@
         <v>400</v>
       </c>
       <c r="D268" s="9" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
     </row>
     <row r="269" spans="3:4" x14ac:dyDescent="0.3">
@@ -7347,7 +7346,7 @@
         <v>400</v>
       </c>
       <c r="D269" s="9" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
     </row>
     <row r="270" spans="3:4" x14ac:dyDescent="0.3">
@@ -7355,7 +7354,7 @@
         <v>400</v>
       </c>
       <c r="D270" s="9" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
     </row>
     <row r="271" spans="3:4" x14ac:dyDescent="0.3">
@@ -7363,7 +7362,7 @@
         <v>400</v>
       </c>
       <c r="D271" s="9" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
     </row>
     <row r="272" spans="3:4" x14ac:dyDescent="0.3">
@@ -7371,7 +7370,7 @@
         <v>400</v>
       </c>
       <c r="D272" s="9" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
     </row>
     <row r="273" spans="3:4" x14ac:dyDescent="0.3">
@@ -7379,7 +7378,7 @@
         <v>400</v>
       </c>
       <c r="D273" s="9" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
     </row>
     <row r="274" spans="3:4" x14ac:dyDescent="0.3">
@@ -7387,7 +7386,7 @@
         <v>400</v>
       </c>
       <c r="D274" s="9" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
     </row>
     <row r="275" spans="3:4" x14ac:dyDescent="0.3">
@@ -7395,7 +7394,7 @@
         <v>400</v>
       </c>
       <c r="D275" s="9" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
     </row>
     <row r="276" spans="3:4" x14ac:dyDescent="0.3">
@@ -7403,7 +7402,7 @@
         <v>400</v>
       </c>
       <c r="D276" s="9" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
     </row>
     <row r="277" spans="3:4" x14ac:dyDescent="0.3">
@@ -7411,7 +7410,7 @@
         <v>400</v>
       </c>
       <c r="D277" s="9" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
     </row>
     <row r="278" spans="3:4" x14ac:dyDescent="0.3">
@@ -7419,7 +7418,7 @@
         <v>400</v>
       </c>
       <c r="D278" s="9" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
     </row>
     <row r="279" spans="3:4" x14ac:dyDescent="0.3">
@@ -7427,7 +7426,7 @@
         <v>400</v>
       </c>
       <c r="D279" s="9" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
     </row>
     <row r="280" spans="3:4" x14ac:dyDescent="0.3">
@@ -7435,7 +7434,7 @@
         <v>400</v>
       </c>
       <c r="D280" s="9" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
     </row>
     <row r="281" spans="3:4" x14ac:dyDescent="0.3">
@@ -7443,7 +7442,7 @@
         <v>400</v>
       </c>
       <c r="D281" s="9" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
     </row>
     <row r="282" spans="3:4" x14ac:dyDescent="0.3">
@@ -7451,7 +7450,7 @@
         <v>400</v>
       </c>
       <c r="D282" s="9" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
     </row>
     <row r="283" spans="3:4" x14ac:dyDescent="0.3">
@@ -7459,7 +7458,7 @@
         <v>400</v>
       </c>
       <c r="D283" s="9" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
     </row>
     <row r="284" spans="3:4" x14ac:dyDescent="0.3">
@@ -7467,7 +7466,7 @@
         <v>400</v>
       </c>
       <c r="D284" s="9" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
     </row>
     <row r="285" spans="3:4" x14ac:dyDescent="0.3">
@@ -7475,7 +7474,7 @@
         <v>400</v>
       </c>
       <c r="D285" s="9" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
     </row>
     <row r="286" spans="3:4" x14ac:dyDescent="0.3">
@@ -7483,7 +7482,7 @@
         <v>400</v>
       </c>
       <c r="D286" s="9" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="287" spans="3:4" x14ac:dyDescent="0.3">
@@ -7491,7 +7490,7 @@
         <v>400</v>
       </c>
       <c r="D287" s="9" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="288" spans="3:4" x14ac:dyDescent="0.3">
@@ -7499,7 +7498,7 @@
         <v>400</v>
       </c>
       <c r="D288" s="9" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
     </row>
     <row r="289" spans="3:4" x14ac:dyDescent="0.3">
@@ -7507,7 +7506,7 @@
         <v>400</v>
       </c>
       <c r="D289" s="9" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
     </row>
     <row r="290" spans="3:4" x14ac:dyDescent="0.3">
@@ -7515,7 +7514,7 @@
         <v>400</v>
       </c>
       <c r="D290" s="9" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
     </row>
     <row r="291" spans="3:4" x14ac:dyDescent="0.3">
@@ -7523,7 +7522,7 @@
         <v>400</v>
       </c>
       <c r="D291" s="9" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
     </row>
     <row r="292" spans="3:4" x14ac:dyDescent="0.3">
@@ -7531,7 +7530,7 @@
         <v>400</v>
       </c>
       <c r="D292" s="9" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
     </row>
     <row r="293" spans="3:4" x14ac:dyDescent="0.3">
@@ -7539,7 +7538,7 @@
         <v>400</v>
       </c>
       <c r="D293" s="9" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
     </row>
     <row r="294" spans="3:4" x14ac:dyDescent="0.3">
@@ -7547,7 +7546,7 @@
         <v>400</v>
       </c>
       <c r="D294" s="9" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
     </row>
     <row r="295" spans="3:4" x14ac:dyDescent="0.3">
@@ -7555,7 +7554,7 @@
         <v>400</v>
       </c>
       <c r="D295" s="9" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
     </row>
     <row r="296" spans="3:4" x14ac:dyDescent="0.3">
@@ -7563,7 +7562,7 @@
         <v>400</v>
       </c>
       <c r="D296" s="9" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
     </row>
     <row r="297" spans="3:4" x14ac:dyDescent="0.3">
@@ -7571,7 +7570,7 @@
         <v>400</v>
       </c>
       <c r="D297" s="9" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
     </row>
     <row r="298" spans="3:4" x14ac:dyDescent="0.3">
@@ -7579,7 +7578,7 @@
         <v>400</v>
       </c>
       <c r="D298" s="9" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
     </row>
     <row r="299" spans="3:4" x14ac:dyDescent="0.3">
@@ -7587,7 +7586,7 @@
         <v>400</v>
       </c>
       <c r="D299" s="9" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
     </row>
     <row r="300" spans="3:4" x14ac:dyDescent="0.3">
@@ -7595,7 +7594,7 @@
         <v>400</v>
       </c>
       <c r="D300" s="9" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="301" spans="3:4" x14ac:dyDescent="0.3">
@@ -7603,7 +7602,7 @@
         <v>400</v>
       </c>
       <c r="D301" s="9" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
     </row>
     <row r="302" spans="3:4" x14ac:dyDescent="0.3">
@@ -7611,7 +7610,7 @@
         <v>400</v>
       </c>
       <c r="D302" s="9" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="303" spans="3:4" x14ac:dyDescent="0.3">
@@ -7619,7 +7618,7 @@
         <v>400</v>
       </c>
       <c r="D303" s="9" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="304" spans="3:4" x14ac:dyDescent="0.3">
@@ -7627,7 +7626,7 @@
         <v>400</v>
       </c>
       <c r="D304" s="9" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
     </row>
     <row r="305" spans="3:4" x14ac:dyDescent="0.3">
@@ -7635,7 +7634,7 @@
         <v>400</v>
       </c>
       <c r="D305" s="9" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="306" spans="3:4" x14ac:dyDescent="0.3">
@@ -7643,7 +7642,7 @@
         <v>400</v>
       </c>
       <c r="D306" s="9" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
     </row>
     <row r="307" spans="3:4" x14ac:dyDescent="0.3">
@@ -7651,7 +7650,7 @@
         <v>400</v>
       </c>
       <c r="D307" s="9" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
     </row>
     <row r="308" spans="3:4" x14ac:dyDescent="0.3">
@@ -7659,7 +7658,7 @@
         <v>400</v>
       </c>
       <c r="D308" s="9" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
     </row>
     <row r="309" spans="3:4" x14ac:dyDescent="0.3">
@@ -7667,7 +7666,7 @@
         <v>400</v>
       </c>
       <c r="D309" s="9" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="310" spans="3:4" x14ac:dyDescent="0.3">
@@ -7675,7 +7674,7 @@
         <v>400</v>
       </c>
       <c r="D310" s="9" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
     </row>
     <row r="311" spans="3:4" x14ac:dyDescent="0.3">
@@ -7683,7 +7682,7 @@
         <v>400</v>
       </c>
       <c r="D311" s="9" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
     </row>
     <row r="312" spans="3:4" x14ac:dyDescent="0.3">
@@ -7691,7 +7690,7 @@
         <v>400</v>
       </c>
       <c r="D312" s="9" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
     </row>
     <row r="313" spans="3:4" x14ac:dyDescent="0.3">
@@ -7699,7 +7698,7 @@
         <v>400</v>
       </c>
       <c r="D313" s="9" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
     </row>
     <row r="314" spans="3:4" x14ac:dyDescent="0.3">
@@ -7707,7 +7706,7 @@
         <v>400</v>
       </c>
       <c r="D314" s="9" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
     </row>
     <row r="315" spans="3:4" x14ac:dyDescent="0.3">
@@ -7715,7 +7714,7 @@
         <v>400</v>
       </c>
       <c r="D315" s="9" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
     </row>
     <row r="316" spans="3:4" x14ac:dyDescent="0.3">
@@ -7723,7 +7722,7 @@
         <v>400</v>
       </c>
       <c r="D316" s="9" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
     </row>
     <row r="317" spans="3:4" x14ac:dyDescent="0.3">
@@ -7731,7 +7730,7 @@
         <v>400</v>
       </c>
       <c r="D317" s="9" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
     </row>
     <row r="318" spans="3:4" x14ac:dyDescent="0.3">
@@ -7739,7 +7738,7 @@
         <v>400</v>
       </c>
       <c r="D318" s="9" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
     </row>
     <row r="319" spans="3:4" x14ac:dyDescent="0.3">
@@ -7747,7 +7746,7 @@
         <v>400</v>
       </c>
       <c r="D319" s="9" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
     </row>
     <row r="320" spans="3:4" x14ac:dyDescent="0.3">
@@ -7755,7 +7754,7 @@
         <v>401</v>
       </c>
       <c r="D320" s="9" t="s">
-        <v>577</v>
+        <v>549</v>
       </c>
     </row>
     <row r="321" spans="3:4" x14ac:dyDescent="0.3">
@@ -7763,7 +7762,7 @@
         <v>509</v>
       </c>
       <c r="D321" s="9" t="s">
-        <v>269</v>
+        <v>647</v>
       </c>
     </row>
     <row r="322" spans="3:4" x14ac:dyDescent="0.3">
@@ -7771,7 +7770,7 @@
         <v>509</v>
       </c>
       <c r="D322" s="9" t="s">
-        <v>271</v>
+        <v>648</v>
       </c>
     </row>
     <row r="323" spans="3:4" x14ac:dyDescent="0.3">
@@ -7779,7 +7778,7 @@
         <v>509</v>
       </c>
       <c r="D323" s="9" t="s">
-        <v>270</v>
+        <v>649</v>
       </c>
     </row>
     <row r="324" spans="3:4" x14ac:dyDescent="0.3">
@@ -7787,7 +7786,7 @@
         <v>517</v>
       </c>
       <c r="D324" s="9" t="s">
-        <v>601</v>
+        <v>573</v>
       </c>
     </row>
     <row r="325" spans="3:4" x14ac:dyDescent="0.3">
@@ -7795,7 +7794,7 @@
         <v>517</v>
       </c>
       <c r="D325" s="9" t="s">
-        <v>599</v>
+        <v>571</v>
       </c>
     </row>
     <row r="326" spans="3:4" x14ac:dyDescent="0.3">
@@ -7803,7 +7802,7 @@
         <v>517</v>
       </c>
       <c r="D326" s="9" t="s">
-        <v>598</v>
+        <v>570</v>
       </c>
     </row>
     <row r="327" spans="3:4" x14ac:dyDescent="0.3">
@@ -7811,7 +7810,7 @@
         <v>517</v>
       </c>
       <c r="D327" s="9" t="s">
-        <v>600</v>
+        <v>572</v>
       </c>
     </row>
     <row r="328" spans="3:4" x14ac:dyDescent="0.3">
@@ -7819,7 +7818,7 @@
         <v>517</v>
       </c>
       <c r="D328" s="9" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="329" spans="3:4" x14ac:dyDescent="0.3">
@@ -7827,7 +7826,7 @@
         <v>517</v>
       </c>
       <c r="D329" s="9" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="330" spans="3:4" x14ac:dyDescent="0.3">
@@ -7835,7 +7834,7 @@
         <v>517</v>
       </c>
       <c r="D330" s="9" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="331" spans="3:4" x14ac:dyDescent="0.3">
@@ -7843,7 +7842,7 @@
         <v>518</v>
       </c>
       <c r="D331" s="9" t="s">
-        <v>482</v>
+        <v>454</v>
       </c>
     </row>
     <row r="332" spans="3:4" x14ac:dyDescent="0.3">
@@ -7851,7 +7850,7 @@
         <v>518</v>
       </c>
       <c r="D332" s="9" t="s">
-        <v>483</v>
+        <v>455</v>
       </c>
     </row>
     <row r="333" spans="3:4" x14ac:dyDescent="0.3">
@@ -7859,7 +7858,7 @@
         <v>518</v>
       </c>
       <c r="D333" s="9" t="s">
-        <v>485</v>
+        <v>457</v>
       </c>
     </row>
     <row r="334" spans="3:4" x14ac:dyDescent="0.3">
@@ -7867,7 +7866,7 @@
         <v>519</v>
       </c>
       <c r="D334" s="9" t="s">
-        <v>476</v>
+        <v>650</v>
       </c>
     </row>
     <row r="335" spans="3:4" x14ac:dyDescent="0.3">
@@ -7875,7 +7874,7 @@
         <v>519</v>
       </c>
       <c r="D335" s="9" t="s">
-        <v>480</v>
+        <v>651</v>
       </c>
     </row>
     <row r="336" spans="3:4" x14ac:dyDescent="0.3">
@@ -7883,7 +7882,7 @@
         <v>519</v>
       </c>
       <c r="D336" s="9" t="s">
-        <v>477</v>
+        <v>624</v>
       </c>
     </row>
     <row r="337" spans="3:4" x14ac:dyDescent="0.3">
@@ -7891,7 +7890,7 @@
         <v>519</v>
       </c>
       <c r="D337" s="9" t="s">
-        <v>479</v>
+        <v>625</v>
       </c>
     </row>
     <row r="338" spans="3:4" x14ac:dyDescent="0.3">
@@ -7899,7 +7898,7 @@
         <v>519</v>
       </c>
       <c r="D338" s="9" t="s">
-        <v>645</v>
+        <v>652</v>
       </c>
     </row>
     <row r="339" spans="3:4" x14ac:dyDescent="0.3">
@@ -7907,7 +7906,7 @@
         <v>519</v>
       </c>
       <c r="D339" s="9" t="s">
-        <v>647</v>
+        <v>653</v>
       </c>
     </row>
     <row r="340" spans="3:4" x14ac:dyDescent="0.3">
@@ -7915,7 +7914,7 @@
         <v>519</v>
       </c>
       <c r="D340" s="9" t="s">
-        <v>478</v>
+        <v>626</v>
       </c>
     </row>
     <row r="341" spans="3:4" x14ac:dyDescent="0.3">
@@ -7923,7 +7922,7 @@
         <v>519</v>
       </c>
       <c r="D341" s="9" t="s">
-        <v>475</v>
+        <v>452</v>
       </c>
     </row>
     <row r="342" spans="3:4" x14ac:dyDescent="0.3">
@@ -7931,7 +7930,7 @@
         <v>519</v>
       </c>
       <c r="D342" s="9" t="s">
-        <v>646</v>
+        <v>654</v>
       </c>
     </row>
     <row r="343" spans="3:4" x14ac:dyDescent="0.3">
@@ -7939,7 +7938,7 @@
         <v>519</v>
       </c>
       <c r="D343" s="9" t="s">
-        <v>644</v>
+        <v>610</v>
       </c>
     </row>
     <row r="344" spans="3:4" x14ac:dyDescent="0.3">
@@ -7947,7 +7946,7 @@
         <v>750</v>
       </c>
       <c r="D344" s="9" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
     </row>
     <row r="345" spans="3:4" x14ac:dyDescent="0.3">
@@ -7955,7 +7954,7 @@
         <v>750</v>
       </c>
       <c r="D345" s="9" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
     </row>
     <row r="346" spans="3:4" x14ac:dyDescent="0.3">
@@ -7963,7 +7962,7 @@
         <v>750</v>
       </c>
       <c r="D346" s="9" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="347" spans="3:4" x14ac:dyDescent="0.3">
@@ -7971,7 +7970,7 @@
         <v>750</v>
       </c>
       <c r="D347" s="9" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="348" spans="3:4" x14ac:dyDescent="0.3">
@@ -7979,7 +7978,7 @@
         <v>750</v>
       </c>
       <c r="D348" s="9" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
     </row>
     <row r="349" spans="3:4" x14ac:dyDescent="0.3">
@@ -7987,7 +7986,7 @@
         <v>750</v>
       </c>
       <c r="D349" s="9" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
     </row>
     <row r="350" spans="3:4" x14ac:dyDescent="0.3">
@@ -7995,7 +7994,7 @@
         <v>750</v>
       </c>
       <c r="D350" s="9" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="351" spans="3:4" x14ac:dyDescent="0.3">
@@ -8003,7 +8002,7 @@
         <v>750</v>
       </c>
       <c r="D351" s="9" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="352" spans="3:4" x14ac:dyDescent="0.3">
@@ -8011,7 +8010,7 @@
         <v>750</v>
       </c>
       <c r="D352" s="9" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="353" spans="3:4" x14ac:dyDescent="0.3">
@@ -8019,7 +8018,7 @@
         <v>750</v>
       </c>
       <c r="D353" s="9" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="354" spans="3:4" x14ac:dyDescent="0.3">
@@ -8027,7 +8026,7 @@
         <v>750</v>
       </c>
       <c r="D354" s="9" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
     </row>
     <row r="355" spans="3:4" x14ac:dyDescent="0.3">
@@ -8035,7 +8034,7 @@
         <v>750</v>
       </c>
       <c r="D355" s="9" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
     </row>
     <row r="356" spans="3:4" x14ac:dyDescent="0.3">
@@ -8043,7 +8042,7 @@
         <v>750</v>
       </c>
       <c r="D356" s="9" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
     </row>
     <row r="357" spans="3:4" x14ac:dyDescent="0.3">
@@ -8051,7 +8050,7 @@
         <v>750</v>
       </c>
       <c r="D357" s="9" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="358" spans="3:4" x14ac:dyDescent="0.3">
@@ -8059,7 +8058,7 @@
         <v>750</v>
       </c>
       <c r="D358" s="9" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
     </row>
     <row r="359" spans="3:4" x14ac:dyDescent="0.3">
@@ -8067,7 +8066,7 @@
         <v>750</v>
       </c>
       <c r="D359" s="9" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="360" spans="3:4" x14ac:dyDescent="0.3">
@@ -8075,7 +8074,7 @@
         <v>750</v>
       </c>
       <c r="D360" s="9" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="361" spans="3:4" x14ac:dyDescent="0.3">
@@ -8083,7 +8082,7 @@
         <v>750</v>
       </c>
       <c r="D361" s="9" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="362" spans="3:4" x14ac:dyDescent="0.3">
@@ -8091,7 +8090,7 @@
         <v>750</v>
       </c>
       <c r="D362" s="9" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="363" spans="3:4" x14ac:dyDescent="0.3">
@@ -8099,7 +8098,7 @@
         <v>750</v>
       </c>
       <c r="D363" s="9" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="364" spans="3:4" x14ac:dyDescent="0.3">
@@ -8107,7 +8106,7 @@
         <v>750</v>
       </c>
       <c r="D364" s="9" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
     </row>
     <row r="365" spans="3:4" x14ac:dyDescent="0.3">
@@ -8115,7 +8114,7 @@
         <v>750</v>
       </c>
       <c r="D365" s="9" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="366" spans="3:4" x14ac:dyDescent="0.3">
@@ -8123,7 +8122,7 @@
         <v>750</v>
       </c>
       <c r="D366" s="9" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="367" spans="3:4" x14ac:dyDescent="0.3">
@@ -8131,7 +8130,7 @@
         <v>750</v>
       </c>
       <c r="D367" s="9" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="368" spans="3:4" x14ac:dyDescent="0.3">
@@ -8139,7 +8138,7 @@
         <v>750</v>
       </c>
       <c r="D368" s="9" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
     </row>
     <row r="369" spans="3:4" x14ac:dyDescent="0.3">
@@ -8147,7 +8146,7 @@
         <v>750</v>
       </c>
       <c r="D369" s="9" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="370" spans="3:4" x14ac:dyDescent="0.3">
@@ -8155,7 +8154,7 @@
         <v>750</v>
       </c>
       <c r="D370" s="9" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
     </row>
     <row r="371" spans="3:4" x14ac:dyDescent="0.3">
@@ -8163,7 +8162,7 @@
         <v>750</v>
       </c>
       <c r="D371" s="9" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
     </row>
     <row r="372" spans="3:4" x14ac:dyDescent="0.3">
@@ -8171,7 +8170,7 @@
         <v>750</v>
       </c>
       <c r="D372" s="9" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="373" spans="3:4" x14ac:dyDescent="0.3">
@@ -8179,7 +8178,7 @@
         <v>750</v>
       </c>
       <c r="D373" s="9" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
     </row>
     <row r="374" spans="3:4" x14ac:dyDescent="0.3">
@@ -8187,7 +8186,7 @@
         <v>750</v>
       </c>
       <c r="D374" s="9" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="375" spans="3:4" x14ac:dyDescent="0.3">
@@ -8195,7 +8194,7 @@
         <v>750</v>
       </c>
       <c r="D375" s="9" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="376" spans="3:4" x14ac:dyDescent="0.3">
@@ -8203,7 +8202,7 @@
         <v>750</v>
       </c>
       <c r="D376" s="9" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
     </row>
     <row r="377" spans="3:4" x14ac:dyDescent="0.3">
@@ -8211,7 +8210,7 @@
         <v>750</v>
       </c>
       <c r="D377" s="9" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="378" spans="3:4" x14ac:dyDescent="0.3">
@@ -8219,7 +8218,7 @@
         <v>750</v>
       </c>
       <c r="D378" s="9" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
     </row>
     <row r="379" spans="3:4" x14ac:dyDescent="0.3">
@@ -8227,7 +8226,7 @@
         <v>750</v>
       </c>
       <c r="D379" s="9" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
     </row>
     <row r="380" spans="3:4" x14ac:dyDescent="0.3">
@@ -8235,7 +8234,7 @@
         <v>750</v>
       </c>
       <c r="D380" s="9" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="381" spans="3:4" x14ac:dyDescent="0.3">
@@ -8243,7 +8242,7 @@
         <v>750</v>
       </c>
       <c r="D381" s="9" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="382" spans="3:4" x14ac:dyDescent="0.3">
@@ -8251,7 +8250,7 @@
         <v>750</v>
       </c>
       <c r="D382" s="9" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
     </row>
     <row r="383" spans="3:4" x14ac:dyDescent="0.3">
@@ -8259,7 +8258,7 @@
         <v>750</v>
       </c>
       <c r="D383" s="9" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="384" spans="3:4" x14ac:dyDescent="0.3">
@@ -8267,7 +8266,7 @@
         <v>750</v>
       </c>
       <c r="D384" s="9" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
     </row>
     <row r="385" spans="3:4" x14ac:dyDescent="0.3">
@@ -8275,7 +8274,7 @@
         <v>750</v>
       </c>
       <c r="D385" s="9" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="386" spans="3:4" x14ac:dyDescent="0.3">
@@ -8283,7 +8282,7 @@
         <v>750</v>
       </c>
       <c r="D386" s="9" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="387" spans="3:4" x14ac:dyDescent="0.3">
@@ -8291,7 +8290,7 @@
         <v>750</v>
       </c>
       <c r="D387" s="9" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
     <row r="388" spans="3:4" x14ac:dyDescent="0.3">
@@ -8299,7 +8298,7 @@
         <v>750</v>
       </c>
       <c r="D388" s="9" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="389" spans="3:4" x14ac:dyDescent="0.3">
@@ -8307,7 +8306,7 @@
         <v>750</v>
       </c>
       <c r="D389" s="9" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="390" spans="3:4" x14ac:dyDescent="0.3">
@@ -8315,7 +8314,7 @@
         <v>750</v>
       </c>
       <c r="D390" s="9" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
     </row>
     <row r="391" spans="3:4" x14ac:dyDescent="0.3">
@@ -8323,7 +8322,7 @@
         <v>750</v>
       </c>
       <c r="D391" s="9" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="392" spans="3:4" x14ac:dyDescent="0.3">
@@ -8331,7 +8330,7 @@
         <v>750</v>
       </c>
       <c r="D392" s="9" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="393" spans="3:4" x14ac:dyDescent="0.3">
@@ -8339,7 +8338,7 @@
         <v>750</v>
       </c>
       <c r="D393" s="9" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="394" spans="3:4" x14ac:dyDescent="0.3">
@@ -8347,7 +8346,7 @@
         <v>750</v>
       </c>
       <c r="D394" s="9" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="395" spans="3:4" x14ac:dyDescent="0.3">
@@ -8355,7 +8354,7 @@
         <v>750</v>
       </c>
       <c r="D395" s="9" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="396" spans="3:4" x14ac:dyDescent="0.3">
@@ -8363,7 +8362,7 @@
         <v>750</v>
       </c>
       <c r="D396" s="9" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="397" spans="3:4" x14ac:dyDescent="0.3">
@@ -8371,7 +8370,7 @@
         <v>750</v>
       </c>
       <c r="D397" s="9" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
     </row>
     <row r="398" spans="3:4" x14ac:dyDescent="0.3">
@@ -8379,7 +8378,7 @@
         <v>750</v>
       </c>
       <c r="D398" s="9" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="399" spans="3:4" x14ac:dyDescent="0.3">
@@ -8387,7 +8386,7 @@
         <v>750</v>
       </c>
       <c r="D399" s="9" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
     </row>
     <row r="400" spans="3:4" x14ac:dyDescent="0.3">
@@ -8395,7 +8394,7 @@
         <v>750</v>
       </c>
       <c r="D400" s="9" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="401" spans="3:4" x14ac:dyDescent="0.3">
@@ -8403,7 +8402,7 @@
         <v>750</v>
       </c>
       <c r="D401" s="9" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
     </row>
     <row r="402" spans="3:4" x14ac:dyDescent="0.3">
@@ -8411,7 +8410,7 @@
         <v>750</v>
       </c>
       <c r="D402" s="9" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="403" spans="3:4" x14ac:dyDescent="0.3">
@@ -8419,7 +8418,7 @@
         <v>750</v>
       </c>
       <c r="D403" s="9" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
     </row>
     <row r="404" spans="3:4" x14ac:dyDescent="0.3">
@@ -8427,7 +8426,7 @@
         <v>750</v>
       </c>
       <c r="D404" s="9" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="405" spans="3:4" x14ac:dyDescent="0.3">
@@ -8435,7 +8434,7 @@
         <v>750</v>
       </c>
       <c r="D405" s="9" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
     </row>
     <row r="406" spans="3:4" x14ac:dyDescent="0.3">
@@ -8443,7 +8442,7 @@
         <v>750</v>
       </c>
       <c r="D406" s="9" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="407" spans="3:4" x14ac:dyDescent="0.3">
@@ -8451,7 +8450,7 @@
         <v>750</v>
       </c>
       <c r="D407" s="9" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="408" spans="3:4" x14ac:dyDescent="0.3">
@@ -8459,7 +8458,7 @@
         <v>750</v>
       </c>
       <c r="D408" s="9" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="409" spans="3:4" x14ac:dyDescent="0.3">
@@ -8467,7 +8466,7 @@
         <v>750</v>
       </c>
       <c r="D409" s="9" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
     </row>
     <row r="410" spans="3:4" x14ac:dyDescent="0.3">
@@ -8475,7 +8474,7 @@
         <v>750</v>
       </c>
       <c r="D410" s="9" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="411" spans="3:4" x14ac:dyDescent="0.3">
@@ -8483,7 +8482,7 @@
         <v>750</v>
       </c>
       <c r="D411" s="9" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
     </row>
     <row r="412" spans="3:4" x14ac:dyDescent="0.3">
@@ -8491,7 +8490,7 @@
         <v>750</v>
       </c>
       <c r="D412" s="9" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
     </row>
     <row r="413" spans="3:4" x14ac:dyDescent="0.3">
@@ -8499,7 +8498,7 @@
         <v>750</v>
       </c>
       <c r="D413" s="9" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
     </row>
     <row r="414" spans="3:4" x14ac:dyDescent="0.3">
@@ -8507,7 +8506,7 @@
         <v>750</v>
       </c>
       <c r="D414" s="9" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
     </row>
     <row r="415" spans="3:4" x14ac:dyDescent="0.3">
@@ -8515,7 +8514,7 @@
         <v>750</v>
       </c>
       <c r="D415" s="9" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
     </row>
     <row r="416" spans="3:4" x14ac:dyDescent="0.3">
@@ -8523,7 +8522,7 @@
         <v>750</v>
       </c>
       <c r="D416" s="9" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
     </row>
     <row r="417" spans="3:4" x14ac:dyDescent="0.3">
@@ -8531,7 +8530,7 @@
         <v>750</v>
       </c>
       <c r="D417" s="9" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="418" spans="3:4" x14ac:dyDescent="0.3">
@@ -8539,7 +8538,7 @@
         <v>750</v>
       </c>
       <c r="D418" s="9" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
     </row>
     <row r="419" spans="3:4" x14ac:dyDescent="0.3">
@@ -8547,7 +8546,7 @@
         <v>800</v>
       </c>
       <c r="D419" s="9" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
     </row>
     <row r="420" spans="3:4" x14ac:dyDescent="0.3">
@@ -8555,7 +8554,7 @@
         <v>800</v>
       </c>
       <c r="D420" s="9" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
     </row>
     <row r="421" spans="3:4" x14ac:dyDescent="0.3">
@@ -8563,7 +8562,7 @@
         <v>800</v>
       </c>
       <c r="D421" s="9" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="422" spans="3:4" x14ac:dyDescent="0.3">
@@ -8571,7 +8570,7 @@
         <v>800</v>
       </c>
       <c r="D422" s="9" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
     </row>
     <row r="423" spans="3:4" x14ac:dyDescent="0.3">
@@ -8579,7 +8578,7 @@
         <v>800</v>
       </c>
       <c r="D423" s="9" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
     </row>
     <row r="424" spans="3:4" x14ac:dyDescent="0.3">
@@ -8587,7 +8586,7 @@
         <v>800</v>
       </c>
       <c r="D424" s="9" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="425" spans="3:4" x14ac:dyDescent="0.3">
@@ -8595,7 +8594,7 @@
         <v>800</v>
       </c>
       <c r="D425" s="9" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="426" spans="3:4" x14ac:dyDescent="0.3">
@@ -8603,7 +8602,7 @@
         <v>800</v>
       </c>
       <c r="D426" s="9" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="427" spans="3:4" x14ac:dyDescent="0.3">
@@ -8611,7 +8610,7 @@
         <v>800</v>
       </c>
       <c r="D427" s="9" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -8638,7 +8637,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>659</v>
+        <v>621</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>

</xml_diff>